<commit_message>
added testing on artificial data
also comparison with:
- Neural network regression
- Tree regression
- Support Vector regression
</commit_message>
<xml_diff>
--- a/table1.xlsx
+++ b/table1.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Seb/cloud/gfr/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6063E1-EB1C-FA40-8F87-B3696C38632F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="5460" windowWidth="38320" windowHeight="21160"/>
+    <workbookView xWindow="22460" yWindow="0" windowWidth="23620" windowHeight="25920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -91,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,13 +114,79 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF92D050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,14 +202,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -160,83 +234,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3492500" y="1384300"/>
-          <a:ext cx="4737100" cy="1371600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>© 2017 Zheng et al. This is an open access article distributed under the terms of the Creative Commons Attribution License, which permits unrestricted use, distribution, and reproduction in any medium, provided the original author and source are credited.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>http://journals.plos.org/plosone/article?id=10.1371/journal.pone.0180565</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,17 +522,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="13" width="8.83203125" style="2"/>
-    <col min="14" max="18" width="10" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="8.83203125" style="4"/>
+    <col min="3" max="3" width="8.83203125" style="8"/>
+    <col min="4" max="4" width="8.83203125" style="6"/>
+    <col min="5" max="5" width="8.83203125" style="10"/>
+    <col min="6" max="7" width="8.83203125" style="2"/>
+    <col min="8" max="8" width="8.83203125" style="12"/>
+    <col min="9" max="13" width="8.83203125" style="2"/>
+    <col min="14" max="14" width="10" style="13" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10" style="2" customWidth="1"/>
     <col min="19" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -543,16 +550,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -561,7 +568,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -579,13 +586,13 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="14" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -621,16 +628,16 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>13</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
         <v>1.355</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="9">
         <v>35.5</v>
       </c>
       <c r="F2" s="1">
@@ -639,7 +646,7 @@
       <c r="G2" s="1">
         <v>0.751</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="11">
         <v>0.81899999999999995</v>
       </c>
       <c r="I2" s="1">
@@ -657,13 +664,13 @@
       <c r="M2" s="1">
         <v>1.1579999999999999</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="13">
         <v>56.85</v>
       </c>
       <c r="O2" s="2">
         <v>90.18</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="14">
         <v>68.37</v>
       </c>
       <c r="Q2" s="2">
@@ -699,16 +706,16 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>15</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
         <v>1.58</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="9">
         <v>45.5</v>
       </c>
       <c r="F3" s="1">
@@ -717,7 +724,7 @@
       <c r="G3" s="1">
         <v>0.86199999999999999</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="11">
         <v>0.92700000000000005</v>
       </c>
       <c r="I3" s="1">
@@ -735,13 +742,13 @@
       <c r="M3" s="1">
         <v>1.407</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="13">
         <v>74.58</v>
       </c>
       <c r="O3" s="2">
         <v>109.88</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="14">
         <v>70.355999999999995</v>
       </c>
       <c r="Q3" s="2">
@@ -777,16 +784,16 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="7">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>1.365</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="9">
         <v>23.3</v>
       </c>
       <c r="F4" s="1">
@@ -795,7 +802,7 @@
       <c r="G4" s="1">
         <v>0.36699999999999999</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="11">
         <v>0.44</v>
       </c>
       <c r="I4" s="1">
@@ -813,13 +820,13 @@
       <c r="M4" s="1">
         <v>0.92600000000000005</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="13">
         <v>87.69</v>
       </c>
       <c r="O4" s="2">
         <v>81.93</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="14">
         <v>127.998</v>
       </c>
       <c r="Q4" s="2">
@@ -855,16 +862,16 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>14</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
         <v>1.59</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="9">
         <v>43.5</v>
       </c>
       <c r="F5" s="1">
@@ -873,7 +880,7 @@
       <c r="G5" s="1">
         <v>0.54200000000000004</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="11">
         <v>0.61299999999999999</v>
       </c>
       <c r="I5" s="1">
@@ -891,13 +898,13 @@
       <c r="M5" s="1">
         <v>1.377</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="13">
         <v>82.46</v>
       </c>
       <c r="O5" s="2">
         <v>149.11000000000001</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="14">
         <v>107.161</v>
       </c>
       <c r="Q5" s="2">
@@ -933,16 +940,16 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
         <v>0.85</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="9">
         <v>11.35</v>
       </c>
       <c r="F6" s="1">
@@ -951,7 +958,7 @@
       <c r="G6" s="1">
         <v>2.202</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="11">
         <v>2.2450000000000001</v>
       </c>
       <c r="I6" s="1">
@@ -969,13 +976,13 @@
       <c r="M6" s="1">
         <v>0.52100000000000002</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="13">
         <v>28.28</v>
       </c>
       <c r="O6" s="2">
         <v>21.87</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="14">
         <v>15.635999999999999</v>
       </c>
       <c r="Q6" s="2">
@@ -1011,16 +1018,16 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>11</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="7">
         <v>0</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>1.5649999999999999</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="9">
         <v>42.3</v>
       </c>
       <c r="F7" s="1">
@@ -1029,7 +1036,7 @@
       <c r="G7" s="1">
         <v>0.35099999999999998</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="11">
         <v>0.42499999999999999</v>
       </c>
       <c r="I7" s="1">
@@ -1047,13 +1054,13 @@
       <c r="M7" s="1">
         <v>1.3480000000000001</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="13">
         <v>106.64</v>
       </c>
       <c r="O7" s="2">
         <v>190.23</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="14">
         <v>152.13</v>
       </c>
       <c r="Q7" s="2">
@@ -1089,16 +1096,16 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
         <v>0.86499999999999999</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="9">
         <v>14.5</v>
       </c>
       <c r="F8" s="1">
@@ -1107,7 +1114,7 @@
       <c r="G8" s="1">
         <v>0.192</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="11">
         <v>0.26900000000000002</v>
       </c>
       <c r="I8" s="1">
@@ -1125,13 +1132,13 @@
       <c r="M8" s="1">
         <v>0.59899999999999998</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="13">
         <v>133.07</v>
       </c>
       <c r="O8" s="2">
         <v>116.82</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="14">
         <v>132.71299999999999</v>
       </c>
       <c r="Q8" s="2">
@@ -1167,16 +1174,16 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>13</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>0</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>1.4650000000000001</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="9">
         <v>58</v>
       </c>
       <c r="F9" s="1">
@@ -1185,7 +1192,7 @@
       <c r="G9" s="1">
         <v>1.4139999999999999</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="11">
         <v>1.47</v>
       </c>
       <c r="I9" s="1">
@@ -1203,13 +1210,13 @@
       <c r="M9" s="1">
         <v>1.556</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="13">
         <v>40.32</v>
       </c>
       <c r="O9" s="2">
         <v>58.38</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="14">
         <v>41.155999999999999</v>
       </c>
       <c r="Q9" s="2">
@@ -1245,16 +1252,16 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>0</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>0.82</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="9">
         <v>17.7</v>
       </c>
       <c r="F10" s="1">
@@ -1263,7 +1270,7 @@
       <c r="G10" s="1">
         <v>0.20399999999999999</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="11">
         <v>0.28000000000000003</v>
       </c>
       <c r="I10" s="1">
@@ -1281,13 +1288,13 @@
       <c r="M10" s="1">
         <v>0.65300000000000002</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="13">
         <v>105.64</v>
       </c>
       <c r="O10" s="2">
         <v>107.75</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="14">
         <v>120.818</v>
       </c>
       <c r="Q10" s="2">
@@ -1323,16 +1330,16 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>1.383</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="9">
         <v>35.299999999999997</v>
       </c>
       <c r="F11" s="1">
@@ -1341,7 +1348,7 @@
       <c r="G11" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I11" s="1">
@@ -1359,13 +1366,13 @@
       <c r="M11" s="1">
         <v>1.1639999999999999</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="13">
         <v>109.52</v>
       </c>
       <c r="O11" s="2">
         <v>122.26</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="14">
         <v>106.551</v>
       </c>
       <c r="Q11" s="2">
@@ -1401,16 +1408,16 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
         <v>1.4379999999999999</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="9">
         <v>42.5</v>
       </c>
       <c r="F12" s="1">
@@ -1419,7 +1426,7 @@
       <c r="G12" s="1">
         <v>0.29399999999999998</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="11">
         <v>0.36899999999999999</v>
       </c>
       <c r="I12" s="1">
@@ -1437,13 +1444,13 @@
       <c r="M12" s="1">
         <v>1.306</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="13">
         <v>121.73</v>
       </c>
       <c r="O12" s="2">
         <v>174.79</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="14">
         <v>160.83199999999999</v>
       </c>
       <c r="Q12" s="2">
@@ -1479,16 +1486,16 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
         <v>0.875</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="9">
         <v>26</v>
       </c>
       <c r="F13" s="1">
@@ -1497,7 +1504,7 @@
       <c r="G13" s="1">
         <v>0.23799999999999999</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="11">
         <v>0.314</v>
       </c>
       <c r="I13" s="1">
@@ -1515,13 +1522,13 @@
       <c r="M13" s="1">
         <v>0.82399999999999995</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="13">
         <v>144.15</v>
       </c>
       <c r="O13" s="2">
         <v>114.98</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="14">
         <v>115.21</v>
       </c>
       <c r="Q13" s="2">
@@ -1557,16 +1564,16 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>11</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="7">
         <v>0</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="5">
         <v>1.48</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="9">
         <v>47.8</v>
       </c>
       <c r="F14" s="1">
@@ -1575,7 +1582,7 @@
       <c r="G14" s="1">
         <v>0.32800000000000001</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="11">
         <v>0.40300000000000002</v>
       </c>
       <c r="I14" s="1">
@@ -1593,13 +1600,13 @@
       <c r="M14" s="1">
         <v>1.4079999999999999</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="13">
         <v>114.69</v>
       </c>
       <c r="O14" s="2">
         <v>133.25</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="14">
         <v>151.81399999999999</v>
       </c>
       <c r="Q14" s="2">
@@ -1635,16 +1642,16 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>12</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="7">
         <v>0</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="5">
         <v>1.462</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="9">
         <v>54</v>
       </c>
       <c r="F15" s="1">
@@ -1653,7 +1660,7 @@
       <c r="G15" s="1">
         <v>0.41899999999999998</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="11">
         <v>0.49199999999999999</v>
       </c>
       <c r="I15" s="1">
@@ -1671,13 +1678,13 @@
       <c r="M15" s="1">
         <v>1.496</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="13">
         <v>85.36</v>
       </c>
       <c r="O15" s="2">
         <v>134.12</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="14">
         <v>122.82899999999999</v>
       </c>
       <c r="Q15" s="2">
@@ -1713,16 +1720,16 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>9</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5">
         <v>1.3660000000000001</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="9">
         <v>31.5</v>
       </c>
       <c r="F16" s="1">
@@ -1731,7 +1738,7 @@
       <c r="G16" s="1">
         <v>0.36199999999999999</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="11">
         <v>0.436</v>
       </c>
       <c r="I16" s="1">
@@ -1749,13 +1756,13 @@
       <c r="M16" s="1">
         <v>1.0900000000000001</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="13">
         <v>116.1</v>
       </c>
       <c r="O16" s="2">
         <v>138.36000000000001</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="14">
         <v>129.399</v>
       </c>
       <c r="Q16" s="2">
@@ -1791,16 +1798,16 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>6</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="7">
         <v>0</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="5">
         <v>1.1819999999999999</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="9">
         <v>19.399999999999999</v>
       </c>
       <c r="F17" s="1">
@@ -1809,7 +1816,7 @@
       <c r="G17" s="1">
         <v>0.215</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="11">
         <v>0.29099999999999998</v>
       </c>
       <c r="I17" s="1">
@@ -1827,13 +1834,13 @@
       <c r="M17" s="1">
         <v>0.79300000000000004</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="13">
         <v>116.88</v>
       </c>
       <c r="O17" s="2">
         <v>179.59</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="14">
         <v>167.51</v>
       </c>
       <c r="Q17" s="2">
@@ -1869,16 +1876,16 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
         <v>1.788</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="9">
         <v>94</v>
       </c>
       <c r="F18" s="1">
@@ -1887,7 +1894,7 @@
       <c r="G18" s="1">
         <v>0.80300000000000005</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="11">
         <v>0.87</v>
       </c>
       <c r="I18" s="1">
@@ -1905,13 +1912,13 @@
       <c r="M18" s="1">
         <v>2.1829999999999998</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="13">
         <v>72.260000000000005</v>
       </c>
       <c r="O18" s="2">
         <v>124.34</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="14">
         <v>84.912000000000006</v>
       </c>
       <c r="Q18" s="2">
@@ -1947,16 +1954,16 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="3">
         <v>13</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="7">
         <v>0</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="5">
         <v>1.5049999999999999</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="9">
         <v>48</v>
       </c>
       <c r="F19" s="1">
@@ -1965,7 +1972,7 @@
       <c r="G19" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I19" s="1">
@@ -1983,13 +1990,13 @@
       <c r="M19" s="1">
         <v>1.42</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="13">
         <v>88.22</v>
       </c>
       <c r="O19" s="2">
         <v>143.47999999999999</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19" s="14">
         <v>115.95</v>
       </c>
       <c r="Q19" s="2">
@@ -2025,16 +2032,16 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>7</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="7">
         <v>0</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="5">
         <v>1.2649999999999999</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="9">
         <v>21.6</v>
       </c>
       <c r="F20" s="1">
@@ -2043,7 +2050,7 @@
       <c r="G20" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I20" s="1">
@@ -2061,13 +2068,13 @@
       <c r="M20" s="1">
         <v>0.86299999999999999</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="13">
         <v>73.37</v>
       </c>
       <c r="O20" s="2">
         <v>104.24</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="14">
         <v>97.46</v>
       </c>
       <c r="Q20" s="2">
@@ -2103,16 +2110,16 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="3">
         <v>7</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="7">
         <v>0</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="5">
         <v>1.37</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="9">
         <v>29.5</v>
       </c>
       <c r="F21" s="1">
@@ -2121,7 +2128,7 @@
       <c r="G21" s="1">
         <v>0.373</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="11">
         <v>0.44700000000000001</v>
       </c>
       <c r="I21" s="1">
@@ -2139,13 +2146,13 @@
       <c r="M21" s="1">
         <v>1.0529999999999999</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="13">
         <v>120.07</v>
       </c>
       <c r="O21" s="2">
         <v>125.68</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P21" s="14">
         <v>126.55</v>
       </c>
       <c r="Q21" s="2">
@@ -2181,16 +2188,16 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="3">
         <v>10</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="7">
         <v>0</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="5">
         <v>1.407</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="9">
         <v>35.6</v>
       </c>
       <c r="F22" s="1">
@@ -2199,7 +2206,7 @@
       <c r="G22" s="1">
         <v>0.39600000000000002</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="11">
         <v>0.46899999999999997</v>
       </c>
       <c r="I22" s="1">
@@ -2217,13 +2224,13 @@
       <c r="M22" s="1">
         <v>1.177</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22" s="13">
         <v>134.52000000000001</v>
       </c>
       <c r="O22" s="2">
         <v>131.55000000000001</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P22" s="14">
         <v>123.809</v>
       </c>
       <c r="Q22" s="2">
@@ -2259,16 +2266,16 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="3">
         <v>16</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="7">
         <v>0</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="5">
         <v>1.554</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="9">
         <v>50.6</v>
       </c>
       <c r="F23" s="1">
@@ -2277,7 +2284,7 @@
       <c r="G23" s="1">
         <v>0.52</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="11">
         <v>0.59199999999999997</v>
       </c>
       <c r="I23" s="1">
@@ -2295,13 +2302,13 @@
       <c r="M23" s="1">
         <v>1.48</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="13">
         <v>89.59</v>
       </c>
       <c r="O23" s="2">
         <v>121.86</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P23" s="14">
         <v>108.474</v>
       </c>
       <c r="Q23" s="2">
@@ -2337,16 +2344,16 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="3">
         <v>13</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="7">
         <v>0</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="5">
         <v>1.62</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="9">
         <v>59</v>
       </c>
       <c r="F24" s="1">
@@ -2355,7 +2362,7 @@
       <c r="G24" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I24" s="1">
@@ -2373,13 +2380,13 @@
       <c r="M24" s="1">
         <v>1.6339999999999999</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="13">
         <v>73.349999999999994</v>
       </c>
       <c r="O24" s="2">
         <v>157.53</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24" s="14">
         <v>124.81</v>
       </c>
       <c r="Q24" s="2">
@@ -2415,16 +2422,16 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="3">
         <v>14</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="7">
         <v>0</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="5">
         <v>1.573</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="9">
         <v>49.5</v>
       </c>
       <c r="F25" s="1">
@@ -2433,7 +2440,7 @@
       <c r="G25" s="1">
         <v>0.39600000000000002</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="11">
         <v>0.46899999999999997</v>
       </c>
       <c r="I25" s="1">
@@ -2451,13 +2458,13 @@
       <c r="M25" s="1">
         <v>1.4690000000000001</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="13">
         <v>113.47</v>
       </c>
       <c r="O25" s="2">
         <v>159.33000000000001</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P25" s="14">
         <v>138.416</v>
       </c>
       <c r="Q25" s="2">
@@ -2493,16 +2500,16 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="3">
         <v>13</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="7">
         <v>0</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="5">
         <v>1.3859999999999999</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="9">
         <v>30</v>
       </c>
       <c r="F26" s="1">
@@ -2511,7 +2518,7 @@
       <c r="G26" s="1">
         <v>0.81399999999999995</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="11">
         <v>0.88100000000000001</v>
       </c>
       <c r="I26" s="1">
@@ -2529,13 +2536,13 @@
       <c r="M26" s="1">
         <v>1.0680000000000001</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="13">
         <v>44.69</v>
       </c>
       <c r="O26" s="2">
         <v>78.36</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P26" s="14">
         <v>64.989999999999995</v>
       </c>
       <c r="Q26" s="2">
@@ -2571,16 +2578,16 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="3">
         <v>13</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
         <v>1.39</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="9">
         <v>29</v>
       </c>
       <c r="F27" s="1">
@@ -2589,7 +2596,7 @@
       <c r="G27" s="1">
         <v>0.84799999999999998</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="11">
         <v>0.91400000000000003</v>
       </c>
       <c r="I27" s="1">
@@ -2607,13 +2614,13 @@
       <c r="M27" s="1">
         <v>1.0489999999999999</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="13">
         <v>71.680000000000007</v>
       </c>
       <c r="O27" s="2">
         <v>97.76</v>
       </c>
-      <c r="P27" s="2">
+      <c r="P27" s="14">
         <v>62.798999999999999</v>
       </c>
       <c r="Q27" s="2">
@@ -2649,16 +2656,16 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="3">
         <v>11</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="7">
         <v>0</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="5">
         <v>1.3680000000000001</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="9">
         <v>39.200000000000003</v>
       </c>
       <c r="F28" s="1">
@@ -2667,7 +2674,7 @@
       <c r="G28" s="1">
         <v>0.441</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="11">
         <v>0.51400000000000001</v>
       </c>
       <c r="I28" s="1">
@@ -2685,13 +2692,13 @@
       <c r="M28" s="1">
         <v>1.226</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N28" s="13">
         <v>118.45</v>
       </c>
       <c r="O28" s="2">
         <v>116.69</v>
       </c>
-      <c r="P28" s="2">
+      <c r="P28" s="14">
         <v>109.95699999999999</v>
       </c>
       <c r="Q28" s="2">
@@ -2727,16 +2734,16 @@
       <c r="A29" s="1">
         <v>30</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="3">
         <v>13</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
         <v>1.653</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="9">
         <v>40</v>
       </c>
       <c r="F29" s="1">
@@ -2745,7 +2752,7 @@
       <c r="G29" s="1">
         <v>0.373</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="11">
         <v>0.44700000000000001</v>
       </c>
       <c r="I29" s="1">
@@ -2763,13 +2770,13 @@
       <c r="M29" s="1">
         <v>1.3360000000000001</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N29" s="13">
         <v>107.59</v>
       </c>
       <c r="O29" s="2">
         <v>200.61</v>
       </c>
-      <c r="P29" s="2">
+      <c r="P29" s="14">
         <v>152.691</v>
       </c>
       <c r="Q29" s="2">
@@ -2805,16 +2812,16 @@
       <c r="A30" s="1">
         <v>33</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="3">
         <v>14</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="7">
         <v>0</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="5">
         <v>1.494</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="9">
         <v>52</v>
       </c>
       <c r="F30" s="1">
@@ -2823,7 +2830,7 @@
       <c r="G30" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I30" s="1">
@@ -2841,13 +2848,13 @@
       <c r="M30" s="1">
         <v>1.478</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="13">
         <v>109.97</v>
       </c>
       <c r="O30" s="2">
         <v>127.44</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P30" s="14">
         <v>115.102</v>
       </c>
       <c r="Q30" s="2">
@@ -2883,16 +2890,16 @@
       <c r="A31" s="1">
         <v>34</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="3">
         <v>10</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="7">
         <v>0</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="5">
         <v>1.474</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="9">
         <v>36.5</v>
       </c>
       <c r="F31" s="1">
@@ -2901,7 +2908,7 @@
       <c r="G31" s="1">
         <v>0.30499999999999999</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="11">
         <v>0.38</v>
       </c>
       <c r="I31" s="1">
@@ -2919,13 +2926,13 @@
       <c r="M31" s="1">
         <v>1.216</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N31" s="13">
         <v>128.83000000000001</v>
       </c>
       <c r="O31" s="2">
         <v>162.88</v>
       </c>
-      <c r="P31" s="2">
+      <c r="P31" s="14">
         <v>160.03899999999999</v>
       </c>
       <c r="Q31" s="2">
@@ -2961,16 +2968,16 @@
       <c r="A32" s="1">
         <v>35</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="3">
         <v>10</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="7">
         <v>0</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="5">
         <v>1.218</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="9">
         <v>42</v>
       </c>
       <c r="F32" s="1">
@@ -2979,7 +2986,7 @@
       <c r="G32" s="1">
         <v>0.36199999999999999</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="11">
         <v>0.436</v>
       </c>
       <c r="I32" s="1">
@@ -2997,13 +3004,13 @@
       <c r="M32" s="1">
         <v>1.2150000000000001</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N32" s="13">
         <v>84.42</v>
       </c>
       <c r="O32" s="2">
         <v>123.37</v>
       </c>
-      <c r="P32" s="2">
+      <c r="P32" s="14">
         <v>115.379</v>
       </c>
       <c r="Q32" s="2">
@@ -3039,16 +3046,16 @@
       <c r="A33" s="1">
         <v>36</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="3">
         <v>15</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="7">
         <v>0</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="5">
         <v>1.68</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="9">
         <v>65</v>
       </c>
       <c r="F33" s="1">
@@ -3057,7 +3064,7 @@
       <c r="G33" s="1">
         <v>0.57699999999999996</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="11">
         <v>0.64700000000000002</v>
       </c>
       <c r="I33" s="1">
@@ -3075,13 +3082,13 @@
       <c r="M33" s="1">
         <v>1.746</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33" s="13">
         <v>90.33</v>
       </c>
       <c r="O33" s="2">
         <v>123.76</v>
       </c>
-      <c r="P33" s="2">
+      <c r="P33" s="14">
         <v>107.196</v>
       </c>
       <c r="Q33" s="2">
@@ -3117,16 +3124,16 @@
       <c r="A34" s="1">
         <v>37</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="3">
         <v>11</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="7">
         <v>0</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="5">
         <v>1.55</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="9">
         <v>35</v>
       </c>
       <c r="F34" s="1">
@@ -3135,7 +3142,7 @@
       <c r="G34" s="1">
         <v>0.29399999999999998</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="11">
         <v>0.36899999999999999</v>
       </c>
       <c r="I34" s="1">
@@ -3153,13 +3160,13 @@
       <c r="M34" s="1">
         <v>1.212</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N34" s="13">
         <v>102.37</v>
       </c>
       <c r="O34" s="2">
         <v>289.85000000000002</v>
       </c>
-      <c r="P34" s="2">
+      <c r="P34" s="14">
         <v>173.358</v>
       </c>
       <c r="Q34" s="2">
@@ -3195,16 +3202,16 @@
       <c r="A35" s="1">
         <v>38</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="3">
         <v>11</v>
       </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1">
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
         <v>1.4</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="9">
         <v>60.5</v>
       </c>
       <c r="F35" s="1">
@@ -3213,7 +3220,7 @@
       <c r="G35" s="1">
         <v>0.91600000000000004</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="11">
         <v>0.98099999999999998</v>
       </c>
       <c r="I35" s="1">
@@ -3231,13 +3238,13 @@
       <c r="M35" s="1">
         <v>1.5629999999999999</v>
       </c>
-      <c r="N35" s="2">
+      <c r="N35" s="13">
         <v>62.47</v>
       </c>
       <c r="O35" s="2">
         <v>78.239999999999995</v>
       </c>
-      <c r="P35" s="2">
+      <c r="P35" s="14">
         <v>58.948</v>
       </c>
       <c r="Q35" s="2">
@@ -3273,16 +3280,16 @@
       <c r="A36" s="1">
         <v>39</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="3">
         <v>7</v>
       </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="9">
         <v>19</v>
       </c>
       <c r="F36" s="1">
@@ -3291,7 +3298,7 @@
       <c r="G36" s="1">
         <v>0.28299999999999997</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="11">
         <v>0.35799999999999998</v>
       </c>
       <c r="I36" s="1">
@@ -3309,13 +3316,13 @@
       <c r="M36" s="1">
         <v>0.77</v>
       </c>
-      <c r="N36" s="2">
+      <c r="N36" s="13">
         <v>123.34</v>
       </c>
       <c r="O36" s="2">
         <v>137.35</v>
       </c>
-      <c r="P36" s="2">
+      <c r="P36" s="14">
         <v>130.30799999999999</v>
       </c>
       <c r="Q36" s="2">
@@ -3351,16 +3358,16 @@
       <c r="A37" s="1">
         <v>40</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5">
         <v>0.82</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="9">
         <v>10.75</v>
       </c>
       <c r="F37" s="1">
@@ -3369,7 +3376,7 @@
       <c r="G37" s="1">
         <v>0.249</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="11">
         <v>0.32500000000000001</v>
       </c>
       <c r="I37" s="1">
@@ -3387,13 +3394,13 @@
       <c r="M37" s="1">
         <v>0.499</v>
       </c>
-      <c r="N37" s="2">
+      <c r="N37" s="13">
         <v>115.29</v>
       </c>
       <c r="O37" s="2">
         <v>113.91</v>
       </c>
-      <c r="P37" s="2">
+      <c r="P37" s="14">
         <v>104.27200000000001</v>
       </c>
       <c r="Q37" s="2">
@@ -3429,16 +3436,16 @@
       <c r="A38" s="1">
         <v>41</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="3">
         <v>15</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="7">
         <v>0</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="5">
         <v>1.4730000000000001</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="9">
         <v>53</v>
       </c>
       <c r="F38" s="1">
@@ -3447,7 +3454,7 @@
       <c r="G38" s="1">
         <v>0.45200000000000001</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="11">
         <v>0.52500000000000002</v>
       </c>
       <c r="I38" s="1">
@@ -3465,13 +3472,13 @@
       <c r="M38" s="1">
         <v>1.4850000000000001</v>
       </c>
-      <c r="N38" s="2">
+      <c r="N38" s="13">
         <v>96.22</v>
       </c>
       <c r="O38" s="2">
         <v>123.48</v>
       </c>
-      <c r="P38" s="2">
+      <c r="P38" s="14">
         <v>115.88800000000001</v>
       </c>
       <c r="Q38" s="2">
@@ -3507,16 +3514,16 @@
       <c r="A39" s="1">
         <v>42</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="3">
         <v>7</v>
       </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1">
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5">
         <v>1.3540000000000001</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="9">
         <v>29</v>
       </c>
       <c r="F39" s="1">
@@ -3525,7 +3532,7 @@
       <c r="G39" s="1">
         <v>0.35099999999999998</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="11">
         <v>0.42499999999999999</v>
       </c>
       <c r="I39" s="1">
@@ -3543,13 +3550,13 @@
       <c r="M39" s="1">
         <v>1.0389999999999999</v>
       </c>
-      <c r="N39" s="2">
+      <c r="N39" s="13">
         <v>124.35</v>
       </c>
       <c r="O39" s="2">
         <v>134.35</v>
       </c>
-      <c r="P39" s="2">
+      <c r="P39" s="14">
         <v>131.619</v>
       </c>
       <c r="Q39" s="2">
@@ -3585,16 +3592,16 @@
       <c r="A40" s="1">
         <v>43</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="3">
         <v>14</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="7">
         <v>0</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="5">
         <v>1.5309999999999999</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="9">
         <v>49.5</v>
       </c>
       <c r="F40" s="1">
@@ -3603,7 +3610,7 @@
       <c r="G40" s="1">
         <v>0.52</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="11">
         <v>0.59199999999999997</v>
       </c>
       <c r="I40" s="1">
@@ -3621,13 +3628,13 @@
       <c r="M40" s="1">
         <v>1.454</v>
       </c>
-      <c r="N40" s="2">
+      <c r="N40" s="13">
         <v>81.91</v>
       </c>
       <c r="O40" s="2">
         <v>118.15</v>
       </c>
-      <c r="P40" s="2">
+      <c r="P40" s="14">
         <v>106.869</v>
       </c>
       <c r="Q40" s="2">
@@ -3663,16 +3670,16 @@
       <c r="A41" s="1">
         <v>44</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="3">
         <v>14</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="7">
         <v>0</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="5">
         <v>1.4710000000000001</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="9">
         <v>47.4</v>
       </c>
       <c r="F41" s="1">
@@ -3681,7 +3688,7 @@
       <c r="G41" s="1">
         <v>0.43</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="11">
         <v>0.503</v>
       </c>
       <c r="I41" s="1">
@@ -3699,13 +3706,13 @@
       <c r="M41" s="1">
         <v>1.3979999999999999</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N41" s="13">
         <v>96.2</v>
       </c>
       <c r="O41" s="2">
         <v>125.47</v>
       </c>
-      <c r="P41" s="2">
+      <c r="P41" s="14">
         <v>120.851</v>
       </c>
       <c r="Q41" s="2">
@@ -3741,16 +3748,16 @@
       <c r="A42" s="1">
         <v>46</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="3">
         <v>4</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="7">
         <v>0</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="5">
         <v>0.96599999999999997</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="9">
         <v>15</v>
       </c>
       <c r="F42" s="1">
@@ -3759,7 +3766,7 @@
       <c r="G42" s="1">
         <v>0.22600000000000001</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="11">
         <v>0.30299999999999999</v>
       </c>
       <c r="I42" s="1">
@@ -3777,13 +3784,13 @@
       <c r="M42" s="1">
         <v>0.63700000000000001</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N42" s="13">
         <v>102.6</v>
       </c>
       <c r="O42" s="2">
         <v>173.95</v>
       </c>
-      <c r="P42" s="2">
+      <c r="P42" s="14">
         <v>131.86699999999999</v>
       </c>
       <c r="Q42" s="2">
@@ -3819,16 +3826,16 @@
       <c r="A43" s="1">
         <v>47</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="3">
         <v>15</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="7">
         <v>0</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="5">
         <v>1.5</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="9">
         <v>45</v>
       </c>
       <c r="F43" s="1">
@@ -3837,7 +3844,7 @@
       <c r="G43" s="1">
         <v>0.35099999999999998</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="11">
         <v>0.42499999999999999</v>
       </c>
       <c r="I43" s="1">
@@ -3855,13 +3862,13 @@
       <c r="M43" s="1">
         <v>1.37</v>
       </c>
-      <c r="N43" s="2">
+      <c r="N43" s="13">
         <v>114.13</v>
       </c>
       <c r="O43" s="2">
         <v>162.07</v>
       </c>
-      <c r="P43" s="2">
+      <c r="P43" s="14">
         <v>145.81100000000001</v>
       </c>
       <c r="Q43" s="2">
@@ -3897,16 +3904,16 @@
       <c r="A44" s="1">
         <v>48</v>
       </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1">
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5">
         <v>0.75</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="9">
         <v>10.5</v>
       </c>
       <c r="F44" s="1">
@@ -3915,7 +3922,7 @@
       <c r="G44" s="1">
         <v>0.32800000000000001</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44" s="11">
         <v>0.40300000000000002</v>
       </c>
       <c r="I44" s="1">
@@ -3933,13 +3940,13 @@
       <c r="M44" s="1">
         <v>0.47599999999999998</v>
       </c>
-      <c r="N44" s="2">
+      <c r="N44" s="13">
         <v>80.680000000000007</v>
       </c>
       <c r="O44" s="2">
         <v>93.5</v>
       </c>
-      <c r="P44" s="2">
+      <c r="P44" s="14">
         <v>76.933000000000007</v>
       </c>
       <c r="Q44" s="2">
@@ -3975,16 +3982,16 @@
       <c r="A45" s="1">
         <v>49</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="3">
         <v>17</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="7">
         <v>0</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="5">
         <v>1.5649999999999999</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="9">
         <v>57.4</v>
       </c>
       <c r="F45" s="1">
@@ -3993,7 +4000,7 @@
       <c r="G45" s="1">
         <v>0.57699999999999996</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="11">
         <v>0.64700000000000002</v>
       </c>
       <c r="I45" s="1">
@@ -4011,13 +4018,13 @@
       <c r="M45" s="1">
         <v>1.5880000000000001</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="13">
         <v>73.540000000000006</v>
       </c>
       <c r="O45" s="2">
         <v>124.74</v>
       </c>
-      <c r="P45" s="2">
+      <c r="P45" s="14">
         <v>99.858000000000004</v>
       </c>
       <c r="Q45" s="2">
@@ -4053,16 +4060,16 @@
       <c r="A46" s="1">
         <v>50</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="3">
         <v>10</v>
       </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5">
         <v>1.462</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="9">
         <v>49.1</v>
       </c>
       <c r="F46" s="1">
@@ -4071,7 +4078,7 @@
       <c r="G46" s="1">
         <v>0.41899999999999998</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="11">
         <v>0.49199999999999999</v>
       </c>
       <c r="I46" s="1">
@@ -4089,13 +4096,13 @@
       <c r="M46" s="1">
         <v>1.421</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N46" s="13">
         <v>139.16</v>
       </c>
       <c r="O46" s="2">
         <v>129.24</v>
       </c>
-      <c r="P46" s="2">
+      <c r="P46" s="14">
         <v>122.82899999999999</v>
       </c>
       <c r="Q46" s="2">
@@ -4131,16 +4138,16 @@
       <c r="A47" s="1">
         <v>52</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="3">
         <v>12</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="7">
         <v>0</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="5">
         <v>1.476</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="9">
         <v>39.1</v>
       </c>
       <c r="F47" s="1">
@@ -4149,7 +4156,7 @@
       <c r="G47" s="1">
         <v>0.69</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="11">
         <v>0.75800000000000001</v>
       </c>
       <c r="I47" s="1">
@@ -4167,13 +4174,13 @@
       <c r="M47" s="1">
         <v>1.262</v>
       </c>
-      <c r="N47" s="2">
+      <c r="N47" s="13">
         <v>51.58</v>
       </c>
       <c r="O47" s="2">
         <v>101.07</v>
       </c>
-      <c r="P47" s="2">
+      <c r="P47" s="14">
         <v>80.372</v>
       </c>
       <c r="Q47" s="2">
@@ -4209,16 +4216,16 @@
       <c r="A48" s="1">
         <v>53</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="3">
         <v>17</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="7">
         <v>0</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="5">
         <v>1.5680000000000001</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="9">
         <v>48</v>
       </c>
       <c r="F48" s="1">
@@ -4227,7 +4234,7 @@
       <c r="G48" s="1">
         <v>0.27100000000000002</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48" s="11">
         <v>0.34699999999999998</v>
       </c>
       <c r="I48" s="1">
@@ -4245,13 +4252,13 @@
       <c r="M48" s="1">
         <v>1.4430000000000001</v>
       </c>
-      <c r="N48" s="2">
+      <c r="N48" s="13">
         <v>140.28</v>
       </c>
       <c r="O48" s="2">
         <v>158.83000000000001</v>
       </c>
-      <c r="P48" s="2">
+      <c r="P48" s="14">
         <v>186.61</v>
       </c>
       <c r="Q48" s="2">
@@ -4287,16 +4294,16 @@
       <c r="A49" s="1">
         <v>54</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="3">
         <v>10</v>
       </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1">
+      <c r="C49" s="7">
+        <v>1</v>
+      </c>
+      <c r="D49" s="5">
         <v>1.29</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="9">
         <v>27.5</v>
       </c>
       <c r="F49" s="1">
@@ -4305,7 +4312,7 @@
       <c r="G49" s="1">
         <v>0.871</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H49" s="11">
         <v>0.93600000000000005</v>
       </c>
       <c r="I49" s="1">
@@ -4323,13 +4330,13 @@
       <c r="M49" s="1">
         <v>0.99</v>
       </c>
-      <c r="N49" s="2">
+      <c r="N49" s="13">
         <v>45.21</v>
       </c>
       <c r="O49" s="2">
         <v>72.09</v>
       </c>
-      <c r="P49" s="2">
+      <c r="P49" s="14">
         <v>56.896999999999998</v>
       </c>
       <c r="Q49" s="2">
@@ -4365,16 +4372,16 @@
       <c r="A50" s="1">
         <v>55</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="3">
         <v>11</v>
       </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1">
+      <c r="C50" s="7">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5">
         <v>1.3979999999999999</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="9">
         <v>66.400000000000006</v>
       </c>
       <c r="F50" s="1">
@@ -4383,7 +4390,7 @@
       <c r="G50" s="1">
         <v>1.0860000000000001</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50" s="11">
         <v>1.1479999999999999</v>
       </c>
       <c r="I50" s="1">
@@ -4401,13 +4408,13 @@
       <c r="M50" s="1">
         <v>1.6419999999999999</v>
       </c>
-      <c r="N50" s="2">
+      <c r="N50" s="13">
         <v>38.450000000000003</v>
       </c>
       <c r="O50" s="2">
         <v>62.36</v>
       </c>
-      <c r="P50" s="2">
+      <c r="P50" s="14">
         <v>50.308999999999997</v>
       </c>
       <c r="Q50" s="2">
@@ -4443,16 +4450,16 @@
       <c r="A51" s="1">
         <v>56</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="3">
         <v>7</v>
       </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-      <c r="D51" s="1">
+      <c r="C51" s="7">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5">
         <v>1.2030000000000001</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="9">
         <v>27</v>
       </c>
       <c r="F51" s="1">
@@ -4461,7 +4468,7 @@
       <c r="G51" s="1">
         <v>0.43</v>
       </c>
-      <c r="H51" s="1">
+      <c r="H51" s="11">
         <v>0.503</v>
       </c>
       <c r="I51" s="1">
@@ -4479,13 +4486,13 @@
       <c r="M51" s="1">
         <v>0.95399999999999996</v>
       </c>
-      <c r="N51" s="2">
+      <c r="N51" s="13">
         <v>151.27000000000001</v>
       </c>
       <c r="O51" s="2">
         <v>114.69</v>
       </c>
-      <c r="P51" s="2">
+      <c r="P51" s="14">
         <v>98.832999999999998</v>
       </c>
       <c r="Q51" s="2">
@@ -4521,16 +4528,16 @@
       <c r="A52" s="1">
         <v>57</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="3">
         <v>10</v>
       </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1">
+      <c r="C52" s="7">
+        <v>1</v>
+      </c>
+      <c r="D52" s="5">
         <v>1.3320000000000001</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="9">
         <v>29</v>
       </c>
       <c r="F52" s="1">
@@ -4539,7 +4546,7 @@
       <c r="G52" s="1">
         <v>0.53200000000000003</v>
       </c>
-      <c r="H52" s="1">
+      <c r="H52" s="11">
         <v>0.60299999999999998</v>
       </c>
       <c r="I52" s="1">
@@ -4557,13 +4564,13 @@
       <c r="M52" s="1">
         <v>1.032</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N52" s="13">
         <v>98.15</v>
       </c>
       <c r="O52" s="2">
         <v>132.16999999999999</v>
       </c>
-      <c r="P52" s="2">
+      <c r="P52" s="14">
         <v>91.263000000000005</v>
       </c>
       <c r="Q52" s="2">
@@ -4599,16 +4606,16 @@
       <c r="A53" s="1">
         <v>58</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="3">
         <v>10</v>
       </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1">
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+      <c r="D53" s="5">
         <v>1.37</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="9">
         <v>35.5</v>
       </c>
       <c r="F53" s="1">
@@ -4617,7 +4624,7 @@
       <c r="G53" s="1">
         <v>0.373</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H53" s="11">
         <v>0.44700000000000001</v>
       </c>
       <c r="I53" s="1">
@@ -4635,13 +4642,13 @@
       <c r="M53" s="1">
         <v>1.163</v>
       </c>
-      <c r="N53" s="2">
+      <c r="N53" s="13">
         <v>133.61000000000001</v>
       </c>
       <c r="O53" s="2">
         <v>118.95</v>
       </c>
-      <c r="P53" s="2">
+      <c r="P53" s="14">
         <v>126.55</v>
       </c>
       <c r="Q53" s="2">
@@ -4677,16 +4684,16 @@
       <c r="A54" s="1">
         <v>59</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="3">
         <v>3</v>
       </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1">
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+      <c r="D54" s="5">
         <v>0.97599999999999998</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="9">
         <v>16</v>
       </c>
       <c r="F54" s="1">
@@ -4695,7 +4702,7 @@
       <c r="G54" s="1">
         <v>0.317</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H54" s="11">
         <v>0.39200000000000002</v>
       </c>
       <c r="I54" s="1">
@@ -4713,13 +4720,13 @@
       <c r="M54" s="1">
         <v>0.66200000000000003</v>
       </c>
-      <c r="N54" s="2">
+      <c r="N54" s="13">
         <v>76.41</v>
       </c>
       <c r="O54" s="2">
         <v>107.85</v>
       </c>
-      <c r="P54" s="2">
+      <c r="P54" s="14">
         <v>102.959</v>
       </c>
       <c r="Q54" s="2">
@@ -4755,16 +4762,16 @@
       <c r="A55" s="1">
         <v>60</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="3">
         <v>7</v>
       </c>
-      <c r="C55" s="1">
-        <v>1</v>
-      </c>
-      <c r="D55" s="1">
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+      <c r="D55" s="5">
         <v>1.2529999999999999</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="9">
         <v>26.4</v>
       </c>
       <c r="F55" s="1">
@@ -4773,7 +4780,7 @@
       <c r="G55" s="1">
         <v>0.35099999999999998</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H55" s="11">
         <v>0.42499999999999999</v>
       </c>
       <c r="I55" s="1">
@@ -4791,13 +4798,13 @@
       <c r="M55" s="1">
         <v>0.95799999999999996</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N55" s="13">
         <v>101.63</v>
       </c>
       <c r="O55" s="2">
         <v>119.45</v>
       </c>
-      <c r="P55" s="2">
+      <c r="P55" s="14">
         <v>121.801</v>
       </c>
       <c r="Q55" s="2">
@@ -4833,16 +4840,16 @@
       <c r="A56" s="1">
         <v>61</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="3">
         <v>17</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="7">
         <v>0</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="5">
         <v>1.4370000000000001</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="9">
         <v>45.8</v>
       </c>
       <c r="F56" s="1">
@@ -4851,7 +4858,7 @@
       <c r="G56" s="1">
         <v>0.55400000000000005</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H56" s="11">
         <v>0.625</v>
       </c>
       <c r="I56" s="1">
@@ -4869,13 +4876,13 @@
       <c r="M56" s="1">
         <v>1.36</v>
       </c>
-      <c r="N56" s="2">
+      <c r="N56" s="13">
         <v>109.04</v>
       </c>
       <c r="O56" s="2">
         <v>101.26</v>
       </c>
-      <c r="P56" s="2">
+      <c r="P56" s="14">
         <v>94.953999999999994</v>
       </c>
       <c r="Q56" s="2">
@@ -4911,16 +4918,16 @@
       <c r="A57" s="1">
         <v>62</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="3">
         <v>8</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="7">
         <v>0</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="5">
         <v>1.2230000000000001</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="9">
         <v>23.5</v>
       </c>
       <c r="F57" s="1">
@@ -4929,7 +4936,7 @@
       <c r="G57" s="1">
         <v>0.36199999999999999</v>
       </c>
-      <c r="H57" s="1">
+      <c r="H57" s="11">
         <v>0.436</v>
       </c>
       <c r="I57" s="1">
@@ -4947,13 +4954,13 @@
       <c r="M57" s="1">
         <v>0.89100000000000001</v>
       </c>
-      <c r="N57" s="2">
+      <c r="N57" s="13">
         <v>115.06</v>
       </c>
       <c r="O57" s="2">
         <v>114.35</v>
       </c>
-      <c r="P57" s="2">
+      <c r="P57" s="14">
         <v>115.85299999999999</v>
       </c>
       <c r="Q57" s="2">
@@ -4989,16 +4996,16 @@
       <c r="A58" s="1">
         <v>63</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="3">
         <v>13</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="7">
         <v>0</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="5">
         <v>1.6639999999999999</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="9">
         <v>50</v>
       </c>
       <c r="F58" s="1">
@@ -5007,7 +5014,7 @@
       <c r="G58" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H58" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I58" s="1">
@@ -5025,13 +5032,13 @@
       <c r="M58" s="1">
         <v>1.5109999999999999</v>
       </c>
-      <c r="N58" s="2">
+      <c r="N58" s="13">
         <v>103.73</v>
       </c>
       <c r="O58" s="2">
         <v>147.1</v>
       </c>
-      <c r="P58" s="2">
+      <c r="P58" s="14">
         <v>128.19999999999999</v>
       </c>
       <c r="Q58" s="2">
@@ -5067,16 +5074,16 @@
       <c r="A59" s="1">
         <v>64</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="3">
         <v>2</v>
       </c>
-      <c r="C59" s="1">
-        <v>1</v>
-      </c>
-      <c r="D59" s="1">
-        <v>1</v>
-      </c>
-      <c r="E59" s="1">
+      <c r="C59" s="7">
+        <v>1</v>
+      </c>
+      <c r="D59" s="5">
+        <v>1</v>
+      </c>
+      <c r="E59" s="9">
         <v>15</v>
       </c>
       <c r="F59" s="1">
@@ -5085,7 +5092,7 @@
       <c r="G59" s="1">
         <v>0.96199999999999997</v>
       </c>
-      <c r="H59" s="1">
+      <c r="H59" s="11">
         <v>1.0249999999999999</v>
       </c>
       <c r="I59" s="1">
@@ -5103,13 +5110,13 @@
       <c r="M59" s="1">
         <v>0.64600000000000002</v>
       </c>
-      <c r="N59" s="2">
+      <c r="N59" s="13">
         <v>25.34</v>
       </c>
       <c r="O59" s="2">
         <v>50.65</v>
       </c>
-      <c r="P59" s="2">
+      <c r="P59" s="14">
         <v>40.279000000000003</v>
       </c>
       <c r="Q59" s="2">
@@ -5145,16 +5152,16 @@
       <c r="A60" s="1">
         <v>66</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="3">
         <v>8</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="7">
         <v>0</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="5">
         <v>1.278</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="9">
         <v>27.5</v>
       </c>
       <c r="F60" s="1">
@@ -5163,7 +5170,7 @@
       <c r="G60" s="1">
         <v>0.249</v>
       </c>
-      <c r="H60" s="1">
+      <c r="H60" s="11">
         <v>0.32500000000000001</v>
       </c>
       <c r="I60" s="1">
@@ -5181,13 +5188,13 @@
       <c r="M60" s="1">
         <v>0.98599999999999999</v>
       </c>
-      <c r="N60" s="2">
+      <c r="N60" s="13">
         <v>105.39</v>
       </c>
       <c r="O60" s="2">
         <v>126.81</v>
       </c>
-      <c r="P60" s="2">
+      <c r="P60" s="14">
         <v>162.512</v>
       </c>
       <c r="Q60" s="2">
@@ -5223,16 +5230,16 @@
       <c r="A61" s="1">
         <v>67</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="3">
         <v>15</v>
       </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1">
+      <c r="C61" s="7">
+        <v>1</v>
+      </c>
+      <c r="D61" s="5">
         <v>1.5369999999999999</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="9">
         <v>44.5</v>
       </c>
       <c r="F61" s="1">
@@ -5241,7 +5248,7 @@
       <c r="G61" s="1">
         <v>0.498</v>
       </c>
-      <c r="H61" s="1">
+      <c r="H61" s="11">
         <v>0.56899999999999995</v>
       </c>
       <c r="I61" s="1">
@@ -5259,13 +5266,13 @@
       <c r="M61" s="1">
         <v>1.375</v>
       </c>
-      <c r="N61" s="2">
+      <c r="N61" s="13">
         <v>124.35</v>
       </c>
       <c r="O61" s="2">
         <v>169.87</v>
       </c>
-      <c r="P61" s="2">
+      <c r="P61" s="14">
         <v>111.47799999999999</v>
       </c>
       <c r="Q61" s="2">
@@ -5301,16 +5308,16 @@
       <c r="A62" s="1">
         <v>68</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="3">
         <v>4</v>
       </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
-      <c r="D62" s="1">
+      <c r="C62" s="7">
+        <v>1</v>
+      </c>
+      <c r="D62" s="5">
         <v>0.99299999999999999</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="9">
         <v>14.3</v>
       </c>
       <c r="F62" s="1">
@@ -5319,7 +5326,7 @@
       <c r="G62" s="1">
         <v>0.317</v>
       </c>
-      <c r="H62" s="1">
+      <c r="H62" s="11">
         <v>0.39200000000000002</v>
       </c>
       <c r="I62" s="1">
@@ -5337,13 +5344,13 @@
       <c r="M62" s="1">
         <v>0.628</v>
       </c>
-      <c r="N62" s="2">
+      <c r="N62" s="13">
         <v>143.16</v>
       </c>
       <c r="O62" s="2">
         <v>112.28</v>
       </c>
-      <c r="P62" s="2">
+      <c r="P62" s="14">
         <v>104.752</v>
       </c>
       <c r="Q62" s="2">
@@ -5379,16 +5386,16 @@
       <c r="A63" s="1">
         <v>69</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="3">
         <v>14</v>
       </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="1">
+      <c r="C63" s="7">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5">
         <v>1.4530000000000001</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="9">
         <v>40.299999999999997</v>
       </c>
       <c r="F63" s="1">
@@ -5397,7 +5404,7 @@
       <c r="G63" s="1">
         <v>0.36199999999999999</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H63" s="11">
         <v>0.436</v>
       </c>
       <c r="I63" s="1">
@@ -5415,13 +5422,13 @@
       <c r="M63" s="1">
         <v>1.2749999999999999</v>
       </c>
-      <c r="N63" s="2">
+      <c r="N63" s="13">
         <v>70.41</v>
       </c>
       <c r="O63" s="2">
         <v>169.68</v>
       </c>
-      <c r="P63" s="2">
+      <c r="P63" s="14">
         <v>137.63999999999999</v>
       </c>
       <c r="Q63" s="2">
@@ -5457,16 +5464,16 @@
       <c r="A64" s="1">
         <v>70</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="3">
         <v>11</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="7">
         <v>0</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="5">
         <v>1.5740000000000001</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="9">
         <v>35.799999999999997</v>
       </c>
       <c r="F64" s="1">
@@ -5475,7 +5482,7 @@
       <c r="G64" s="1">
         <v>1.1539999999999999</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H64" s="11">
         <v>1.214</v>
       </c>
       <c r="I64" s="1">
@@ -5493,13 +5500,13 @@
       <c r="M64" s="1">
         <v>1.2350000000000001</v>
       </c>
-      <c r="N64" s="2">
+      <c r="N64" s="13">
         <v>42.45</v>
       </c>
       <c r="O64" s="2">
         <v>46.38</v>
       </c>
-      <c r="P64" s="2">
+      <c r="P64" s="14">
         <v>53.53</v>
       </c>
       <c r="Q64" s="2">
@@ -5535,16 +5542,16 @@
       <c r="A65" s="1">
         <v>72</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="3">
         <v>12</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="7">
         <v>0</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="5">
         <v>1.405</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="9">
         <v>35.5</v>
       </c>
       <c r="F65" s="1">
@@ -5553,7 +5560,7 @@
       <c r="G65" s="1">
         <v>0.32800000000000001</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H65" s="11">
         <v>0.40300000000000002</v>
       </c>
       <c r="I65" s="1">
@@ -5571,13 +5578,13 @@
       <c r="M65" s="1">
         <v>1.175</v>
       </c>
-      <c r="N65" s="2">
+      <c r="N65" s="13">
         <v>120.25</v>
       </c>
       <c r="O65" s="2">
         <v>158.86000000000001</v>
       </c>
-      <c r="P65" s="2">
+      <c r="P65" s="14">
         <v>144.12100000000001</v>
       </c>
       <c r="Q65" s="2">
@@ -5613,16 +5620,16 @@
       <c r="A66" s="1">
         <v>73</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="3">
         <v>13</v>
       </c>
-      <c r="C66" s="1">
-        <v>1</v>
-      </c>
-      <c r="D66" s="1">
+      <c r="C66" s="7">
+        <v>1</v>
+      </c>
+      <c r="D66" s="5">
         <v>1.381</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="9">
         <v>59.6</v>
       </c>
       <c r="F66" s="1">
@@ -5631,7 +5638,7 @@
       <c r="G66" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H66" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I66" s="1">
@@ -5649,13 +5656,13 @@
       <c r="M66" s="1">
         <v>1.542</v>
       </c>
-      <c r="N66" s="2">
+      <c r="N66" s="13">
         <v>106.69</v>
       </c>
       <c r="O66" s="2">
         <v>185.81</v>
       </c>
-      <c r="P66" s="2">
+      <c r="P66" s="14">
         <v>106.39700000000001</v>
       </c>
       <c r="Q66" s="2">
@@ -5691,16 +5698,16 @@
       <c r="A67" s="1">
         <v>74</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="3">
         <v>10</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="7">
         <v>0</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="5">
         <v>1.3759999999999999</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="9">
         <v>25</v>
       </c>
       <c r="F67" s="1">
@@ -5709,7 +5716,7 @@
       <c r="G67" s="1">
         <v>0.32800000000000001</v>
       </c>
-      <c r="H67" s="1">
+      <c r="H67" s="11">
         <v>0.40300000000000002</v>
       </c>
       <c r="I67" s="1">
@@ -5727,13 +5734,13 @@
       <c r="M67" s="1">
         <v>0.96499999999999997</v>
       </c>
-      <c r="N67" s="2">
+      <c r="N67" s="13">
         <v>100.01</v>
       </c>
       <c r="O67" s="2">
         <v>163.16999999999999</v>
       </c>
-      <c r="P67" s="2">
+      <c r="P67" s="14">
         <v>141.14599999999999</v>
       </c>
       <c r="Q67" s="2">
@@ -5769,16 +5776,16 @@
       <c r="A68" s="1">
         <v>75</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="3">
         <v>10</v>
       </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1">
+      <c r="C68" s="7">
+        <v>1</v>
+      </c>
+      <c r="D68" s="5">
         <v>1.468</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="9">
         <v>34.5</v>
       </c>
       <c r="F68" s="1">
@@ -5787,7 +5794,7 @@
       <c r="G68" s="1">
         <v>0.317</v>
       </c>
-      <c r="H68" s="1">
+      <c r="H68" s="11">
         <v>0.39200000000000002</v>
       </c>
       <c r="I68" s="1">
@@ -5805,13 +5812,13 @@
       <c r="M68" s="1">
         <v>1.177</v>
       </c>
-      <c r="N68" s="2">
+      <c r="N68" s="13">
         <v>144.52000000000001</v>
       </c>
       <c r="O68" s="2">
         <v>162.21</v>
       </c>
-      <c r="P68" s="2">
+      <c r="P68" s="14">
         <v>154.86000000000001</v>
       </c>
       <c r="Q68" s="2">
@@ -5847,16 +5854,16 @@
       <c r="A69" s="1">
         <v>76</v>
       </c>
-      <c r="B69" s="1">
-        <v>1</v>
-      </c>
-      <c r="C69" s="1">
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+      <c r="C69" s="7">
         <v>0</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="5">
         <v>0.71</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="9">
         <v>12.1</v>
       </c>
       <c r="F69" s="1">
@@ -5865,7 +5872,7 @@
       <c r="G69" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="H69" s="1">
+      <c r="H69" s="11">
         <v>0.53600000000000003</v>
       </c>
       <c r="I69" s="1">
@@ -5883,13 +5890,13 @@
       <c r="M69" s="1">
         <v>0.503</v>
       </c>
-      <c r="N69" s="2">
+      <c r="N69" s="13">
         <v>66.069999999999993</v>
       </c>
       <c r="O69" s="2">
         <v>67.69</v>
       </c>
-      <c r="P69" s="2">
+      <c r="P69" s="14">
         <v>54.701000000000001</v>
       </c>
       <c r="Q69" s="2">
@@ -5925,16 +5932,16 @@
       <c r="A70" s="1">
         <v>77</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="3">
         <v>13</v>
       </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="1">
+      <c r="C70" s="7">
+        <v>1</v>
+      </c>
+      <c r="D70" s="5">
         <v>1.371</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="9">
         <v>32.799999999999997</v>
       </c>
       <c r="F70" s="1">
@@ -5943,7 +5950,7 @@
       <c r="G70" s="1">
         <v>1.5720000000000001</v>
       </c>
-      <c r="H70" s="1">
+      <c r="H70" s="11">
         <v>1.6259999999999999</v>
       </c>
       <c r="I70" s="1">
@@ -5961,13 +5968,13 @@
       <c r="M70" s="1">
         <v>1.115</v>
       </c>
-      <c r="N70" s="2">
+      <c r="N70" s="13">
         <v>39.380000000000003</v>
       </c>
       <c r="O70" s="2">
         <v>55.83</v>
       </c>
-      <c r="P70" s="2">
+      <c r="P70" s="14">
         <v>34.826999999999998</v>
       </c>
       <c r="Q70" s="2">
@@ -6003,16 +6010,16 @@
       <c r="A71" s="1">
         <v>78</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="3">
         <v>13</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71" s="7">
         <v>0</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="5">
         <v>1.55</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="9">
         <v>30</v>
       </c>
       <c r="F71" s="1">
@@ -6021,7 +6028,7 @@
       <c r="G71" s="1">
         <v>0.28299999999999997</v>
       </c>
-      <c r="H71" s="1">
+      <c r="H71" s="11">
         <v>0.35799999999999998</v>
       </c>
       <c r="I71" s="1">
@@ -6039,13 +6046,13 @@
       <c r="M71" s="1">
         <v>1.1160000000000001</v>
       </c>
-      <c r="N71" s="2">
+      <c r="N71" s="13">
         <v>95.21</v>
       </c>
       <c r="O71" s="2">
         <v>171.28</v>
       </c>
-      <c r="P71" s="2">
+      <c r="P71" s="14">
         <v>178.74100000000001</v>
       </c>
       <c r="Q71" s="2">
@@ -6081,16 +6088,16 @@
       <c r="A72" s="1">
         <v>81</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="3">
         <v>11</v>
       </c>
-      <c r="C72" s="1">
-        <v>1</v>
-      </c>
-      <c r="D72" s="1">
+      <c r="C72" s="7">
+        <v>1</v>
+      </c>
+      <c r="D72" s="5">
         <v>1.2569999999999999</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="9">
         <v>27.4</v>
       </c>
       <c r="F72" s="1">
@@ -6099,7 +6106,7 @@
       <c r="G72" s="1">
         <v>0.70099999999999996</v>
       </c>
-      <c r="H72" s="1">
+      <c r="H72" s="11">
         <v>0.77</v>
       </c>
       <c r="I72" s="1">
@@ -6117,13 +6124,13 @@
       <c r="M72" s="1">
         <v>0.97799999999999998</v>
       </c>
-      <c r="N72" s="2">
+      <c r="N72" s="13">
         <v>154.58000000000001</v>
       </c>
       <c r="O72" s="2">
         <v>98.57</v>
       </c>
-      <c r="P72" s="2">
+      <c r="P72" s="14">
         <v>67.457999999999998</v>
       </c>
       <c r="Q72" s="2">
@@ -6159,16 +6166,16 @@
       <c r="A73" s="1">
         <v>82</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="3">
         <v>14</v>
       </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="1">
+      <c r="C73" s="7">
+        <v>1</v>
+      </c>
+      <c r="D73" s="5">
         <v>1.66</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="9">
         <v>78</v>
       </c>
       <c r="F73" s="1">
@@ -6177,7 +6184,7 @@
       <c r="G73" s="1">
         <v>0.55400000000000005</v>
       </c>
-      <c r="H73" s="1">
+      <c r="H73" s="11">
         <v>0.625</v>
       </c>
       <c r="I73" s="1">
@@ -6195,13 +6202,13 @@
       <c r="M73" s="1">
         <v>1.917</v>
       </c>
-      <c r="N73" s="2">
+      <c r="N73" s="13">
         <v>153.47999999999999</v>
       </c>
       <c r="O73" s="2">
         <v>158.07</v>
       </c>
-      <c r="P73" s="2">
+      <c r="P73" s="14">
         <v>109.68899999999999</v>
       </c>
       <c r="Q73" s="2">
@@ -6237,16 +6244,16 @@
       <c r="A74" s="1">
         <v>83</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="3">
         <v>15</v>
       </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="1">
+      <c r="C74" s="7">
+        <v>1</v>
+      </c>
+      <c r="D74" s="5">
         <v>1.8</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="9">
         <v>63.5</v>
       </c>
       <c r="F74" s="1">
@@ -6255,7 +6262,7 @@
       <c r="G74" s="1">
         <v>1.26</v>
       </c>
-      <c r="H74" s="1">
+      <c r="H74" s="11">
         <v>1.319</v>
       </c>
       <c r="I74" s="1">
@@ -6273,13 +6280,13 @@
       <c r="M74" s="1">
         <v>1.772</v>
       </c>
-      <c r="N74" s="2">
+      <c r="N74" s="13">
         <v>64.34</v>
       </c>
       <c r="O74" s="2">
         <v>98.59</v>
       </c>
-      <c r="P74" s="2">
+      <c r="P74" s="14">
         <v>56.365000000000002</v>
       </c>
       <c r="Q74" s="2">
@@ -6315,16 +6322,16 @@
       <c r="A75" s="1">
         <v>84</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="3">
         <v>15</v>
       </c>
-      <c r="C75" s="1">
-        <v>1</v>
-      </c>
-      <c r="D75" s="1">
+      <c r="C75" s="7">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5">
         <v>1.72</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="9">
         <v>79</v>
       </c>
       <c r="F75" s="1">
@@ -6333,7 +6340,7 @@
       <c r="G75" s="1">
         <v>0.97299999999999998</v>
       </c>
-      <c r="H75" s="1">
+      <c r="H75" s="11">
         <v>1.036</v>
       </c>
       <c r="I75" s="1">
@@ -6351,13 +6358,13 @@
       <c r="M75" s="1">
         <v>1.9570000000000001</v>
       </c>
-      <c r="N75" s="2">
+      <c r="N75" s="13">
         <v>90.27</v>
       </c>
       <c r="O75" s="2">
         <v>104.37</v>
       </c>
-      <c r="P75" s="2">
+      <c r="P75" s="14">
         <v>68.537000000000006</v>
       </c>
       <c r="Q75" s="2">
@@ -6393,16 +6400,16 @@
       <c r="A76" s="1">
         <v>85</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="3">
         <v>15</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="7">
         <v>0</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="5">
         <v>1.56</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="9">
         <v>46.5</v>
       </c>
       <c r="F76" s="1">
@@ -6411,7 +6418,7 @@
       <c r="G76" s="1">
         <v>0.48599999999999999</v>
       </c>
-      <c r="H76" s="1">
+      <c r="H76" s="11">
         <v>0.55800000000000005</v>
       </c>
       <c r="I76" s="1">
@@ -6429,13 +6436,13 @@
       <c r="M76" s="1">
         <v>1.4159999999999999</v>
       </c>
-      <c r="N76" s="2">
+      <c r="N76" s="13">
         <v>107.15</v>
       </c>
       <c r="O76" s="2">
         <v>176.39</v>
       </c>
-      <c r="P76" s="2">
+      <c r="P76" s="14">
         <v>115.4</v>
       </c>
       <c r="Q76" s="2">
@@ -6471,16 +6478,16 @@
       <c r="A77" s="1">
         <v>86</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="3">
         <v>15</v>
       </c>
-      <c r="C77" s="1">
-        <v>1</v>
-      </c>
-      <c r="D77" s="1">
+      <c r="C77" s="7">
+        <v>1</v>
+      </c>
+      <c r="D77" s="5">
         <v>1.7</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="9">
         <v>60</v>
       </c>
       <c r="F77" s="1">
@@ -6489,7 +6496,7 @@
       <c r="G77" s="1">
         <v>0.65600000000000003</v>
       </c>
-      <c r="H77" s="1">
+      <c r="H77" s="11">
         <v>0.72499999999999998</v>
       </c>
       <c r="I77" s="1">
@@ -6507,13 +6514,13 @@
       <c r="M77" s="1">
         <v>1.68</v>
       </c>
-      <c r="N77" s="2">
+      <c r="N77" s="13">
         <v>132.11000000000001</v>
       </c>
       <c r="O77" s="2">
         <v>181.41</v>
       </c>
-      <c r="P77" s="2">
+      <c r="P77" s="14">
         <v>96.828000000000003</v>
       </c>
       <c r="Q77" s="2">
@@ -6549,16 +6556,16 @@
       <c r="A78" s="1">
         <v>88</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="3">
         <v>16</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="7">
         <v>0</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="5">
         <v>1.55</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="9">
         <v>47</v>
       </c>
       <c r="F78" s="1">
@@ -6567,7 +6574,7 @@
       <c r="G78" s="1">
         <v>0.27100000000000002</v>
       </c>
-      <c r="H78" s="1">
+      <c r="H78" s="11">
         <v>0.34699999999999998</v>
       </c>
       <c r="I78" s="1">
@@ -6585,13 +6592,13 @@
       <c r="M78" s="1">
         <v>1.421</v>
       </c>
-      <c r="N78" s="2">
+      <c r="N78" s="13">
         <v>163.46</v>
       </c>
       <c r="O78" s="2">
         <v>235.5</v>
       </c>
-      <c r="P78" s="2">
+      <c r="P78" s="14">
         <v>184.46799999999999</v>
       </c>
       <c r="Q78" s="2">
@@ -6627,16 +6634,16 @@
       <c r="A79" s="1">
         <v>89</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="3">
         <v>16</v>
       </c>
-      <c r="C79" s="1">
-        <v>1</v>
-      </c>
-      <c r="D79" s="1">
+      <c r="C79" s="7">
+        <v>1</v>
+      </c>
+      <c r="D79" s="5">
         <v>1.74</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79" s="9">
         <v>57</v>
       </c>
       <c r="F79" s="1">
@@ -6645,7 +6652,7 @@
       <c r="G79" s="1">
         <v>0.67900000000000005</v>
       </c>
-      <c r="H79" s="1">
+      <c r="H79" s="11">
         <v>0.747</v>
       </c>
       <c r="I79" s="1">
@@ -6663,13 +6670,13 @@
       <c r="M79" s="1">
         <v>1.65</v>
       </c>
-      <c r="N79" s="2">
+      <c r="N79" s="13">
         <v>135.34</v>
       </c>
       <c r="O79" s="2">
         <v>147.53</v>
       </c>
-      <c r="P79" s="2">
+      <c r="P79" s="14">
         <v>96.156999999999996</v>
       </c>
       <c r="Q79" s="2">
@@ -6705,16 +6712,16 @@
       <c r="A80" s="1">
         <v>90</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="3">
         <v>16</v>
       </c>
-      <c r="C80" s="1">
-        <v>1</v>
-      </c>
-      <c r="D80" s="1">
+      <c r="C80" s="7">
+        <v>1</v>
+      </c>
+      <c r="D80" s="5">
         <v>1.75</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80" s="9">
         <v>58</v>
       </c>
       <c r="F80" s="1">
@@ -6723,7 +6730,7 @@
       <c r="G80" s="1">
         <v>1.0860000000000001</v>
       </c>
-      <c r="H80" s="1">
+      <c r="H80" s="11">
         <v>1.1479999999999999</v>
       </c>
       <c r="I80" s="1">
@@ -6741,13 +6748,13 @@
       <c r="M80" s="1">
         <v>1.669</v>
       </c>
-      <c r="N80" s="2">
+      <c r="N80" s="13">
         <v>53.32</v>
       </c>
       <c r="O80" s="2">
         <v>94.19</v>
       </c>
-      <c r="P80" s="2">
+      <c r="P80" s="14">
         <v>62.975999999999999</v>
       </c>
       <c r="Q80" s="2">
@@ -6783,16 +6790,16 @@
       <c r="A81" s="1">
         <v>91</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="3">
         <v>16</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="7">
         <v>0</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="5">
         <v>1.71</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81" s="9">
         <v>59</v>
       </c>
       <c r="F81" s="1">
@@ -6801,7 +6808,7 @@
       <c r="G81" s="1">
         <v>0.57699999999999996</v>
       </c>
-      <c r="H81" s="1">
+      <c r="H81" s="11">
         <v>0.64700000000000002</v>
       </c>
       <c r="I81" s="1">
@@ -6819,13 +6826,13 @@
       <c r="M81" s="1">
         <v>1.669</v>
       </c>
-      <c r="N81" s="2">
+      <c r="N81" s="13">
         <v>99.89</v>
       </c>
       <c r="O81" s="2">
         <v>163.02000000000001</v>
       </c>
-      <c r="P81" s="2">
+      <c r="P81" s="14">
         <v>109.11</v>
       </c>
       <c r="Q81" s="2">
@@ -6861,16 +6868,16 @@
       <c r="A82" s="1">
         <v>92</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="3">
         <v>17</v>
       </c>
-      <c r="C82" s="1">
-        <v>1</v>
-      </c>
-      <c r="D82" s="1">
+      <c r="C82" s="7">
+        <v>1</v>
+      </c>
+      <c r="D82" s="5">
         <v>1.77</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="9">
         <v>58.5</v>
       </c>
       <c r="F82" s="1">
@@ -6879,7 +6886,7 @@
       <c r="G82" s="1">
         <v>1.6459999999999999</v>
       </c>
-      <c r="H82" s="1">
+      <c r="H82" s="11">
         <v>1.698</v>
       </c>
       <c r="I82" s="1">
@@ -6897,13 +6904,13 @@
       <c r="M82" s="1">
         <v>1.6839999999999999</v>
       </c>
-      <c r="N82" s="2">
+      <c r="N82" s="13">
         <v>51.83</v>
       </c>
       <c r="O82" s="2">
         <v>71.14</v>
       </c>
-      <c r="P82" s="2">
+      <c r="P82" s="14">
         <v>43.048999999999999</v>
       </c>
       <c r="Q82" s="2">
@@ -6939,16 +6946,16 @@
       <c r="A83" s="1">
         <v>93</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="3">
         <v>17</v>
       </c>
-      <c r="C83" s="1">
-        <v>1</v>
-      </c>
-      <c r="D83" s="1">
+      <c r="C83" s="7">
+        <v>1</v>
+      </c>
+      <c r="D83" s="5">
         <v>1.81</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="9">
         <v>72</v>
       </c>
       <c r="F83" s="1">
@@ -6957,7 +6964,7 @@
       <c r="G83" s="1">
         <v>0.94799999999999995</v>
       </c>
-      <c r="H83" s="1">
+      <c r="H83" s="11">
         <v>1.012</v>
       </c>
       <c r="I83" s="1">
@@ -6975,13 +6982,13 @@
       <c r="M83" s="1">
         <v>1.9</v>
       </c>
-      <c r="N83" s="2">
+      <c r="N83" s="13">
         <v>99.71</v>
       </c>
       <c r="O83" s="2">
         <v>117.92</v>
       </c>
-      <c r="P83" s="2">
+      <c r="P83" s="14">
         <v>73.867000000000004</v>
       </c>
       <c r="Q83" s="2">
@@ -7017,16 +7024,16 @@
       <c r="A84" s="1">
         <v>94</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="3">
         <v>17</v>
       </c>
-      <c r="C84" s="1">
-        <v>1</v>
-      </c>
-      <c r="D84" s="1">
+      <c r="C84" s="7">
+        <v>1</v>
+      </c>
+      <c r="D84" s="5">
         <v>1.69</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E84" s="9">
         <v>49</v>
       </c>
       <c r="F84" s="1">
@@ -7035,7 +7042,7 @@
       <c r="G84" s="1">
         <v>0.71299999999999997</v>
       </c>
-      <c r="H84" s="1">
+      <c r="H84" s="11">
         <v>0.78100000000000003</v>
       </c>
       <c r="I84" s="1">
@@ -7053,13 +7060,13 @@
       <c r="M84" s="1">
         <v>1.5029999999999999</v>
       </c>
-      <c r="N84" s="2">
+      <c r="N84" s="13">
         <v>94.43</v>
       </c>
       <c r="O84" s="2">
         <v>166.03</v>
       </c>
-      <c r="P84" s="2">
+      <c r="P84" s="14">
         <v>89.403000000000006</v>
       </c>
       <c r="Q84" s="2">
@@ -7095,16 +7102,16 @@
       <c r="A85" s="1">
         <v>95</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="3">
         <v>17</v>
       </c>
-      <c r="C85" s="1">
-        <v>1</v>
-      </c>
-      <c r="D85" s="1">
+      <c r="C85" s="7">
+        <v>1</v>
+      </c>
+      <c r="D85" s="5">
         <v>1.76</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85" s="9">
         <v>65</v>
       </c>
       <c r="F85" s="1">
@@ -7113,7 +7120,7 @@
       <c r="G85" s="1">
         <v>1.222</v>
       </c>
-      <c r="H85" s="1">
+      <c r="H85" s="11">
         <v>1.2809999999999999</v>
       </c>
       <c r="I85" s="1">
@@ -7131,13 +7138,13 @@
       <c r="M85" s="1">
         <v>1.7789999999999999</v>
       </c>
-      <c r="N85" s="2">
+      <c r="N85" s="13">
         <v>76.16</v>
       </c>
       <c r="O85" s="2">
         <v>100.86</v>
       </c>
-      <c r="P85" s="2">
+      <c r="P85" s="14">
         <v>56.738999999999997</v>
       </c>
       <c r="Q85" s="2">
@@ -7173,16 +7180,16 @@
       <c r="A86" s="1">
         <v>96</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="3">
         <v>18</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="7">
         <v>0</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="5">
         <v>1.57</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="9">
         <v>56.5</v>
       </c>
       <c r="F86" s="1">
@@ -7191,7 +7198,7 @@
       <c r="G86" s="1">
         <v>0.41199999999999998</v>
       </c>
-      <c r="H86" s="1">
+      <c r="H86" s="11">
         <v>0.48499999999999999</v>
       </c>
       <c r="I86" s="1">
@@ -7209,13 +7216,13 @@
       <c r="M86" s="1">
         <v>1.5760000000000001</v>
       </c>
-      <c r="N86" s="2">
+      <c r="N86" s="13">
         <v>116.63</v>
       </c>
       <c r="O86" s="2">
         <v>131.61000000000001</v>
       </c>
-      <c r="P86" s="2">
+      <c r="P86" s="14">
         <v>133.71700000000001</v>
       </c>
       <c r="Q86" s="2">
@@ -7251,16 +7258,16 @@
       <c r="A87" s="1">
         <v>97</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="3">
         <v>18</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="7">
         <v>0</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="5">
         <v>1.62</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87" s="9">
         <v>49</v>
       </c>
       <c r="F87" s="1">
@@ -7269,7 +7276,7 @@
       <c r="G87" s="1">
         <v>0.64500000000000002</v>
       </c>
-      <c r="H87" s="1">
+      <c r="H87" s="11">
         <v>0.71399999999999997</v>
       </c>
       <c r="I87" s="1">
@@ -7287,13 +7294,13 @@
       <c r="M87" s="1">
         <v>1.478</v>
       </c>
-      <c r="N87" s="2">
+      <c r="N87" s="13">
         <v>89.87</v>
       </c>
       <c r="O87" s="2">
         <v>138.18</v>
       </c>
-      <c r="P87" s="2">
+      <c r="P87" s="14">
         <v>93.707999999999998</v>
       </c>
       <c r="Q87" s="2">
@@ -7329,16 +7336,16 @@
       <c r="A88" s="1">
         <v>98</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="3">
         <v>18</v>
       </c>
-      <c r="C88" s="1">
-        <v>1</v>
-      </c>
-      <c r="D88" s="1">
+      <c r="C88" s="7">
+        <v>1</v>
+      </c>
+      <c r="D88" s="5">
         <v>1.75</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E88" s="9">
         <v>60</v>
       </c>
       <c r="F88" s="1">
@@ -7347,7 +7354,7 @@
       <c r="G88" s="1">
         <v>1.9339999999999999</v>
       </c>
-      <c r="H88" s="1">
+      <c r="H88" s="11">
         <v>1.982</v>
       </c>
       <c r="I88" s="1">
@@ -7365,13 +7372,13 @@
       <c r="M88" s="1">
         <v>1.7</v>
       </c>
-      <c r="N88" s="2">
+      <c r="N88" s="13">
         <v>54.3</v>
       </c>
       <c r="O88" s="2">
         <v>63.34</v>
       </c>
-      <c r="P88" s="2">
+      <c r="P88" s="14">
         <v>36.472000000000001</v>
       </c>
       <c r="Q88" s="2">
@@ -7406,6 +7413,5 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>